<commit_message>
test NG on ders rapor avec rapor alma
</commit_message>
<xml_diff>
--- a/target/test-classes/ULKELER.xlsx
+++ b/target/test-classes/ULKELER.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isimsiz\Documents\ExelDosya\"/>
     </mc:Choice>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>ULKELER</t>
   </si>
@@ -133,12 +133,19 @@
   </si>
   <si>
     <t>Mercedes</t>
+  </si>
+  <si>
+    <t>NUFUS</t>
+  </si>
+  <si>
+    <t>83 Milyon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -505,7 +512,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303FAEA0-B941-4376-AAA5-E80E2FE5FEA9}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -513,11 +520,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="33.42578125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="22.28515625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="19.42578125" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="21.5703125" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="33.42578125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -530,7 +537,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -630,17 +639,6 @@
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>